<commit_message>
NumMethods: passed lw4, lw7
</commit_message>
<xml_diff>
--- a/Numerical methods/LW4/LW4.xlsx
+++ b/Numerical methods/LW4/LW4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Numerical methods\LW4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\studies\Numerical methods\LW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC9F340-302B-4EE9-B80D-E919EEC07054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D3ECF6-C8EF-4CDD-905A-620C4251DB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Линейные преобразования" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -304,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -313,19 +310,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -335,8 +330,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -623,33 +618,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>5.2403000000000004</v>
       </c>
@@ -681,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>-1.4360999999999999</v>
       </c>
@@ -713,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>5.1886000000000001</v>
       </c>
@@ -745,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>5.4817</v>
       </c>
@@ -777,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>-2.5373000000000001</v>
       </c>
@@ -809,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>1</v>
       </c>
@@ -841,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>0</v>
       </c>
@@ -873,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>0</v>
       </c>
@@ -905,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>0</v>
       </c>
@@ -937,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0</v>
       </c>
@@ -969,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>1</v>
       </c>
@@ -1001,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>0</v>
       </c>
@@ -1033,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0</v>
       </c>
@@ -1065,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>0</v>
       </c>
@@ -1097,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>0</v>
       </c>
@@ -1129,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1</v>
       </c>
@@ -1161,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>0</v>
       </c>
@@ -1193,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>0</v>
       </c>
@@ -1225,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>0</v>
       </c>
@@ -1257,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>0</v>
       </c>
@@ -1289,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1321,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>0</v>
       </c>
@@ -1353,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>0</v>
       </c>
@@ -1385,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>0</v>
       </c>
@@ -1417,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>0</v>
       </c>
@@ -1449,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>1</v>
       </c>
@@ -1481,7 +1476,7 @@
         <v>-0.22406999999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>0</v>
       </c>
@@ -1513,7 +1508,7 @@
         <v>0.29547000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>0</v>
       </c>
@@ -1545,7 +1540,7 @@
         <v>-6.2869999999999995E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>0</v>
       </c>
@@ -1577,7 +1572,7 @@
         <v>-1.069E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1609,23 +1604,23 @@
         <v>0.23569999999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B38" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5" t="s">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B39" cm="1">
         <f t="array" ref="B39:F43">MMULT(B2:F6,G32:K36)</f>
         <v>1.0000298949999997</v>
@@ -1659,7 +1654,7 @@
         <v>-3.5514999999985974E-4</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>-2.5732000000056043E-5</v>
       </c>
@@ -1691,7 +1686,7 @@
         <v>1.46949999999757E-4</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>8.9687000000004957E-5</v>
       </c>
@@ -1723,7 +1718,7 @@
         <v>2.6564199999998261E-4</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>-6.6403000000048173E-5</v>
       </c>
@@ -1755,7 +1750,7 @@
         <v>-1.1671999999979948E-5</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>-3.8690000001007085E-6</v>
       </c>
@@ -1787,7 +1782,7 @@
         <v>0.99972706099999975</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>25</v>
       </c>
@@ -1816,7 +1811,7 @@
         <v>4.6956522526943052E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C46">
         <v>21.936199999999999</v>
       </c>
@@ -1828,7 +1823,7 @@
         <v>6.5588304716968082E-3</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C47">
         <v>115.9093</v>
       </c>
@@ -1840,7 +1835,7 @@
         <v>7.6514608128519512E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C48">
         <v>36.249299999999998</v>
       </c>
@@ -1852,7 +1847,7 @@
         <v>-4.4537447043417444E-2</v>
       </c>
     </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C49">
         <v>47.121200000000002</v>
       </c>
@@ -1879,23 +1874,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3599B854-98ED-432D-8A24-3A9175064B13}">
   <dimension ref="A2:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" customWidth="1"/>
-    <col min="34" max="34" width="11.28515625" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" customWidth="1"/>
+    <col min="26" max="26" width="10.81640625" customWidth="1"/>
+    <col min="30" max="30" width="10.453125" customWidth="1"/>
+    <col min="34" max="34" width="11.26953125" customWidth="1"/>
+    <col min="35" max="35" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>5.2403000000000004</v>
       </c>
@@ -1911,14 +1906,31 @@
       <c r="F2">
         <v>-1.3241000000000001</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="U2" cm="1">
+        <f t="array" ref="U2:V3">MMULT(AH9:AI10,D9:E10)</f>
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>8.3266726846886741E-17</v>
+      </c>
+      <c r="X2" cm="1">
+        <f t="array" ref="X2:Z4">MMULT(AH12:AJ14,D12:F14)</f>
+        <v>0.99999999999999933</v>
+      </c>
+      <c r="Y2">
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="Z2">
+        <v>-2.2204460492503131E-16</v>
+      </c>
+      <c r="AH2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AI2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>-1.4360999999999999</v>
       </c>
@@ -1934,14 +1946,29 @@
       <c r="F3">
         <v>-1.2518</v>
       </c>
-      <c r="AH3" s="11" t="s">
+      <c r="U3">
+        <v>2.2204460492503131E-16</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>2.2204460492503131E-16</v>
+      </c>
+      <c r="Y3">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="Z3">
+        <v>6.6613381477509392E-16</v>
+      </c>
+      <c r="AH3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AI3" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>5.1886000000000001</v>
       </c>
@@ -1957,8 +1984,17 @@
       <c r="F4">
         <v>-9.3440999999999992</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>5.4817</v>
       </c>
@@ -1975,7 +2011,7 @@
         <v>4.4775</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>-2.5373000000000001</v>
       </c>
@@ -1992,82 +2028,82 @@
         <v>-2.7947000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="9" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8" t="s">
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="10" t="s">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10" t="s">
+      <c r="S8" s="6"/>
+      <c r="T8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U8" s="10"/>
-      <c r="V8" s="9" t="s">
+      <c r="U8" s="6"/>
+      <c r="V8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="9" t="s">
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="9" t="s">
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="10"/>
-      <c r="AN8" s="9" t="s">
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="9"/>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="10"/>
-      <c r="AT8" s="9" t="s">
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AU8" s="9"/>
-      <c r="AV8" s="9"/>
-      <c r="AW8" s="9"/>
-      <c r="AX8" s="9"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="AU8" s="14"/>
+      <c r="AV8" s="14"/>
+      <c r="AW8" s="14"/>
+      <c r="AX8" s="14"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="B9" s="15">
         <v>2</v>
       </c>
       <c r="D9">
@@ -2123,9 +2159,9 @@
         <v>8.3266726846886741E-17</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="17"/>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15"/>
       <c r="D10">
         <v>-1.4360999999999999</v>
       </c>
@@ -2153,13 +2189,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="13">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11">
         <v>3</v>
       </c>
       <c r="D12">
@@ -2235,9 +2271,9 @@
         <v>-2.2204460492503131E-16</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
+      <c r="B13" s="12"/>
       <c r="D13">
         <v>-1.4360999999999999</v>
       </c>
@@ -2290,9 +2326,9 @@
         <v>6.6613381477509392E-16</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="15"/>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13"/>
       <c r="D14">
         <v>5.1886000000000001</v>
       </c>
@@ -2332,13 +2368,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11">
         <v>4</v>
       </c>
       <c r="D16">
@@ -2435,9 +2470,9 @@
         <v>-1.1102230246251565E-16</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
+    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="B17" s="12"/>
       <c r="D17">
         <v>-1.4360999999999999</v>
       </c>
@@ -2508,9 +2543,9 @@
         <v>-6.6613381477509392E-16</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="14"/>
+    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
+      <c r="B18" s="12"/>
       <c r="D18">
         <v>5.1886000000000001</v>
       </c>
@@ -2581,9 +2616,9 @@
         <v>-3.6082248300317588E-16</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="15"/>
+    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13"/>
       <c r="D19">
         <v>5.4817</v>
       </c>
@@ -2635,13 +2670,12 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="13">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="B21" s="11">
         <v>5</v>
       </c>
       <c r="D21">
@@ -2759,9 +2793,9 @@
         <v>3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="14"/>
+    <row r="22" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="12"/>
       <c r="D22">
         <v>-1.4360999999999999</v>
       </c>
@@ -2850,9 +2884,9 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="14"/>
+    <row r="23" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="12"/>
       <c r="D23">
         <v>5.1886000000000001</v>
       </c>
@@ -2941,9 +2975,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="14"/>
+    <row r="24" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A24" s="5"/>
+      <c r="B24" s="12"/>
       <c r="D24">
         <v>5.4817</v>
       </c>
@@ -3032,9 +3066,9 @@
         <v>6.9388939039072284E-18</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="15"/>
+    <row r="25" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A25" s="5"/>
+      <c r="B25" s="13"/>
       <c r="D25">
         <v>-2.5373000000000001</v>
       </c>
@@ -3098,10 +3132,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -3123,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="C28">
         <v>21.936199999999999</v>
@@ -3136,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.35">
       <c r="C29">
         <v>115.9093</v>
       </c>
@@ -3148,8 +3182,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
       <c r="C30">
         <v>36.249299999999998</v>
       </c>
@@ -3161,8 +3195,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
       <c r="C31">
         <v>47.121200000000002</v>
       </c>
@@ -3174,28 +3208,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+    <row r="32" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AN8:AR8"/>
+    <mergeCell ref="AT8:AX8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B21:B25"/>
     <mergeCell ref="J8:N8"/>
     <mergeCell ref="V8:Z8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AH8:AL8"/>
     <mergeCell ref="D8:H8"/>
-    <mergeCell ref="AN8:AR8"/>
-    <mergeCell ref="AT8:AX8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>